<commit_message>
Update tech attributes calculation
- correction of t-type 1 (car) and 2 (moto). In the tech attributes calculations  it was the other way around.
- correction of name of the csv file
- addition of the time update procedure
- calculation of time score
- scale for population introduced as an input in the interface. It is easier to change in this way.
</commit_message>
<xml_diff>
--- a/Netlogo/CSV Variables.xlsx
+++ b/Netlogo/CSV Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dff41cb20eb6b5f4/Documentos/GitHub/Cali-Transport-Sim/Netlogo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{FA0EB150-E30F-4106-A7DE-225D42B20E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A62A667-1CAC-4108-A4F5-29146E8104AD}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{FA0EB150-E30F-4106-A7DE-225D42B20E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{784E7FD7-BF44-43B9-8918-93491980917F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9A5CB342-ACF8-451B-8941-267385EFFA84}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="152">
   <si>
     <t>Description</t>
   </si>
@@ -594,6 +594,12 @@
   </si>
   <si>
     <t>Price increase moto</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>6.6</t>
   </si>
 </sst>
 </file>
@@ -1018,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABEF978-0631-4DC7-BB63-B9DEBA5ACD8D}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+      <selection activeCell="C94" sqref="C94:C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1920,6 +1926,48 @@
         <v>25</v>
       </c>
     </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>61</v>
+      </c>
+      <c r="B94" t="s">
+        <v>125</v>
+      </c>
+      <c r="C94" s="4">
+        <v>136</v>
+      </c>
+      <c r="D94" s="8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>62</v>
+      </c>
+      <c r="B95" t="s">
+        <v>126</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D95" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>63</v>
+      </c>
+      <c r="B96" t="s">
+        <v>127</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D96" s="8">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
addition of graphs and monitors
</commit_message>
<xml_diff>
--- a/Netlogo/CSV Variables.xlsx
+++ b/Netlogo/CSV Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathl\Documents\GitHub\Cali-Transport-Sim\Netlogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F90F64-1095-4941-B7A3-5472E268F9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D118FDE-037C-42AF-9627-F0D749BC9AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9A5CB342-ACF8-451B-8941-267385EFFA84}"/>
   </bookViews>
@@ -864,7 +864,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,7 +895,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="5">
-        <v>0.48</v>
+        <v>0.72</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -910,7 +910,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="5">
-        <v>0.432</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -925,7 +925,7 @@
         <v>42</v>
       </c>
       <c r="C4" s="5">
-        <v>0.378</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="D4" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
Update reading probabilities for modes from the CSV file
</commit_message>
<xml_diff>
--- a/Netlogo/CSV Variables.xlsx
+++ b/Netlogo/CSV Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portatil\Documents\GitHub\Cali-Transport-Sim\Netlogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88331133-5388-485D-A52D-12AE4FD2093E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9753AF-DF58-42CA-B04A-EB278BCE6D12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890" xr2:uid="{9A5CB342-ACF8-451B-8941-267385EFFA84}"/>
   </bookViews>
@@ -24,62 +24,12 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Portatil</author>
-  </authors>
-  <commentList>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{F0EC9D54-E178-4957-A664-E4CE842D146E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Portatil:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Portatil:
-Si se incluye la antigüedad, esta se ajustaría a la actual y se pone a decrecer con los años</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="178">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Eficiencia moto</t>
-  </si>
-  <si>
-    <t>Eficiencia car</t>
-  </si>
-  <si>
-    <t>Emisiones moto por km</t>
-  </si>
-  <si>
-    <t>Emisiones car por km</t>
-  </si>
-  <si>
-    <t>Emisiones público (por persona) por km</t>
-  </si>
-  <si>
     <t>Gasoline price</t>
   </si>
   <si>
@@ -92,15 +42,6 @@
     <t>Accident rate public</t>
   </si>
   <si>
-    <t>Probabilidad de ser víctima de un acto delincuencial en moto</t>
-  </si>
-  <si>
-    <t>Probabilidad de ser víctima de un acto delincuencial en carro</t>
-  </si>
-  <si>
-    <t>Probabilidad de ser víctima de un acto delincuencial en bus</t>
-  </si>
-  <si>
     <t>Speed Motorcycle</t>
   </si>
   <si>
@@ -438,13 +379,193 @@
   </si>
   <si>
     <t>2.5</t>
+  </si>
+  <si>
+    <t>Efficiency of moto (Km/gal)</t>
+  </si>
+  <si>
+    <t>Efficiency of car (Km/gal)</t>
+  </si>
+  <si>
+    <t>Emissions moto per Km</t>
+  </si>
+  <si>
+    <t>Emissions car per Km</t>
+  </si>
+  <si>
+    <t>Emissions public (per person) per km</t>
+  </si>
+  <si>
+    <t>Perception of insecurity in moto</t>
+  </si>
+  <si>
+    <t>Perception of insecurity in car</t>
+  </si>
+  <si>
+    <t>Perception of insecurity in public</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>0.40</t>
+  </si>
+  <si>
+    <t>0.47</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.28</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>0.59</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>Probability for male-social-type-1-car</t>
+  </si>
+  <si>
+    <t>Probability for male-social-type-1-mot</t>
+  </si>
+  <si>
+    <t>Probability for male-social-type-1-pub</t>
+  </si>
+  <si>
+    <t>Probability for male-social-type-2-car</t>
+  </si>
+  <si>
+    <t>Probability for male-social-type-2-mot</t>
+  </si>
+  <si>
+    <t>Probability for male-social-type-2-pub</t>
+  </si>
+  <si>
+    <t>Probability for male-social-type-3-car</t>
+  </si>
+  <si>
+    <t>Probability for male-social-type-3-mot</t>
+  </si>
+  <si>
+    <t>Probability for male-social-type-3-pub</t>
+  </si>
+  <si>
+    <t>Probability for female-social-type-1-car</t>
+  </si>
+  <si>
+    <t>Probability for female-social-type-1-mot</t>
+  </si>
+  <si>
+    <t>Probability for female-social-type-1-pub</t>
+  </si>
+  <si>
+    <t>Probability for female-social-type-2-car</t>
+  </si>
+  <si>
+    <t>Probability for female-social-type-2-mot</t>
+  </si>
+  <si>
+    <t>Probability for female-social-type-2-pub</t>
+  </si>
+  <si>
+    <t>Probability for female-social-type-3-car</t>
+  </si>
+  <si>
+    <t>Probability for female-social-type-3-mot</t>
+  </si>
+  <si>
+    <t>Probability for female-social-type-3-pub</t>
+  </si>
+  <si>
+    <t>prob-m1c</t>
+  </si>
+  <si>
+    <t>prob-m1m</t>
+  </si>
+  <si>
+    <t>prob-m1p</t>
+  </si>
+  <si>
+    <t>prob-m2c</t>
+  </si>
+  <si>
+    <t>prob-m2m</t>
+  </si>
+  <si>
+    <t>prob-m2p</t>
+  </si>
+  <si>
+    <t>prob-m3c</t>
+  </si>
+  <si>
+    <t>prob-m3m</t>
+  </si>
+  <si>
+    <t>prob-m3p</t>
+  </si>
+  <si>
+    <t>prob-f1c</t>
+  </si>
+  <si>
+    <t>prob-f1m</t>
+  </si>
+  <si>
+    <t>prob-f1p</t>
+  </si>
+  <si>
+    <t>prob-f2c</t>
+  </si>
+  <si>
+    <t>prob-f2m</t>
+  </si>
+  <si>
+    <t>prob-f2p</t>
+  </si>
+  <si>
+    <t>prob-f3c</t>
+  </si>
+  <si>
+    <t>prob-f3m</t>
+  </si>
+  <si>
+    <t>prob-f3p</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,19 +586,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -860,17 +968,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABEF978-0631-4DC7-BB63-B9DEBA5ACD8D}">
-  <dimension ref="A1:E54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABEF978-0631-4DC7-BB63-B9DEBA5ACD8D}">
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55:B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="23.125" customWidth="1"/>
+    <col min="2" max="2" width="21.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="8"/>
+    <col min="4" max="4" width="45.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15">
@@ -878,24 +988,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -904,13 +1014,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -919,13 +1029,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D4" s="3">
         <v>2</v>
@@ -934,13 +1044,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D5" s="3">
         <v>3</v>
@@ -948,13 +1058,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D6" s="3">
         <v>4</v>
@@ -962,10 +1072,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -976,13 +1086,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D8" s="3">
         <v>6</v>
@@ -990,13 +1100,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3">
         <v>7</v>
@@ -1004,13 +1114,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3">
         <v>8</v>
@@ -1018,13 +1128,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D11" s="3">
         <v>9</v>
@@ -1032,13 +1142,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D12" s="3">
         <v>10</v>
@@ -1046,13 +1156,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D13" s="3">
         <v>11</v>
@@ -1060,13 +1170,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D14" s="3">
         <v>12</v>
@@ -1074,10 +1184,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5">
         <v>110</v>
@@ -1088,10 +1198,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5">
         <v>38</v>
@@ -1102,10 +1212,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C17" s="5">
         <v>126</v>
@@ -1116,10 +1226,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5">
         <v>204</v>
@@ -1130,10 +1240,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C19" s="5">
         <v>60</v>
@@ -1144,13 +1254,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D20" s="3">
         <v>18</v>
@@ -1158,13 +1268,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D21" s="3">
         <v>19</v>
@@ -1172,13 +1282,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D22" s="3">
         <v>20</v>
@@ -1186,13 +1296,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D23" s="3">
         <v>21</v>
@@ -1200,13 +1310,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D24" s="3">
         <v>22</v>
@@ -1214,13 +1324,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D25" s="3">
         <v>23</v>
@@ -1228,10 +1338,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -1242,10 +1352,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -1256,10 +1366,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C28" s="5">
         <v>1200</v>
@@ -1270,13 +1380,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D29" s="3">
         <v>27</v>
@@ -1284,13 +1394,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D30" s="3">
         <v>28</v>
@@ -1298,10 +1408,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C31" s="8">
         <v>74</v>
@@ -1312,10 +1422,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C32" s="8">
         <v>80</v>
@@ -1326,10 +1436,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C33" s="8">
         <v>60</v>
@@ -1340,10 +1450,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C34" s="8">
         <v>66</v>
@@ -1354,10 +1464,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C35" s="8">
         <v>64</v>
@@ -1368,10 +1478,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C36" s="8">
         <v>73</v>
@@ -1382,10 +1492,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C37" s="8">
         <v>59</v>
@@ -1396,10 +1506,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C38" s="8">
         <v>72</v>
@@ -1410,10 +1520,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C39" s="8">
         <v>72</v>
@@ -1424,10 +1534,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C40" s="8">
         <v>24</v>
@@ -1438,10 +1548,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C41" s="8">
         <v>73</v>
@@ -1452,10 +1562,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C42" s="8">
         <v>73</v>
@@ -1466,10 +1576,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C43" s="8">
         <v>79</v>
@@ -1480,10 +1590,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C44" s="8">
         <v>61</v>
@@ -1494,10 +1604,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C45" s="8">
         <v>70</v>
@@ -1508,10 +1618,10 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C46" s="8">
         <v>68</v>
@@ -1522,10 +1632,10 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C47" s="8">
         <v>68</v>
@@ -1536,10 +1646,10 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C48" s="8">
         <v>81</v>
@@ -1550,10 +1660,10 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C49" s="8">
         <v>82</v>
@@ -1564,10 +1674,10 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C50" s="8">
         <v>83</v>
@@ -1578,10 +1688,10 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C51" s="8">
         <v>62</v>
@@ -1592,13 +1702,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D52" s="3">
         <v>50</v>
@@ -1606,13 +1716,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D53" s="3">
         <v>51</v>
@@ -1620,21 +1730,272 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C54" s="8">
         <v>0</v>
       </c>
       <c r="D54" s="3">
         <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D55" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D56" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>144</v>
+      </c>
+      <c r="B57" t="s">
+        <v>162</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D58" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D59" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D60" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>148</v>
+      </c>
+      <c r="B61" t="s">
+        <v>166</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D61" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>149</v>
+      </c>
+      <c r="B62" t="s">
+        <v>167</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D62" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" t="s">
+        <v>168</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D63" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>151</v>
+      </c>
+      <c r="B64" t="s">
+        <v>169</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D64" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>152</v>
+      </c>
+      <c r="B65" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D65" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>153</v>
+      </c>
+      <c r="B66" t="s">
+        <v>171</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>154</v>
+      </c>
+      <c r="B67" t="s">
+        <v>172</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" t="s">
+        <v>173</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>156</v>
+      </c>
+      <c r="B69" t="s">
+        <v>174</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70" t="s">
+        <v>175</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D70" s="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>158</v>
+      </c>
+      <c r="B71" t="s">
+        <v>176</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" t="s">
+        <v>177</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D72" s="3">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change in cost score calculation
</commit_message>
<xml_diff>
--- a/Netlogo/CSV Variables.xlsx
+++ b/Netlogo/CSV Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portatil\Documents\GitHub\Cali-Transport-Sim\Netlogo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathl\Documents\GitHub\Cali-Transport-Sim\Netlogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD8C15D-6CAD-46C4-A6C2-38B887DCF0DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607E9F1F-9344-43F5-8A7E-7750B7F13A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890" xr2:uid="{9A5CB342-ACF8-451B-8941-267385EFFA84}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{9A5CB342-ACF8-451B-8941-267385EFFA84}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="186">
   <si>
     <t>Description</t>
   </si>
@@ -559,13 +570,37 @@
   </si>
   <si>
     <t>prob-f3p</t>
+  </si>
+  <si>
+    <t>Sec</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Ext-Sec</t>
+  </si>
+  <si>
+    <t>Ext-Cap</t>
+  </si>
+  <si>
+    <t>Ext-Comf</t>
+  </si>
+  <si>
+    <t>Ext-Cost</t>
+  </si>
+  <si>
+    <t>Ext-Acc</t>
+  </si>
+  <si>
+    <t>comfort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -587,13 +622,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -608,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -634,7 +690,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,6 +725,319 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>564758</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>73134</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>79439</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{248A9787-0610-1B9E-8731-6A83716C1AE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="564758" y="14856948"/>
+          <a:ext cx="3545511" cy="1865157"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>613695</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>73963</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F984A096-4CFB-401C-DF4A-4DC6D7E69EE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1547446" y="17021908"/>
+          <a:ext cx="1600339" cy="1234547"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>650630</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>15679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681244</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>80117</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BE7A4C1-457F-A11E-2801-00DDCD23CB99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3182815" y="17037587"/>
+          <a:ext cx="1552709" cy="1234547"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>720969</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>11723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>33401</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>74255</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AF073B0-303D-92D6-AA08-F5443CEC443A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4777154" y="17033631"/>
+          <a:ext cx="1588907" cy="1223116"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>744416</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>17584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>186113</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>80899</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4596C1A-B7BA-F505-89B9-2BCAB0DFB5AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="744416" y="18780369"/>
+          <a:ext cx="3482642" cy="1808002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>627185</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>606492</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>117550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3666680D-1C20-477A-E147-BE86389CBF6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4683370" y="20773293"/>
+          <a:ext cx="3025402" cy="1979467"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>365320</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>136721</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>605215</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>110379</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64E6A077-24A6-E3C0-D8E0-E5E96531999B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="365320" y="24895859"/>
+          <a:ext cx="3528365" cy="2095682"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -969,21 +1357,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABEF978-0631-4DC7-BB63-B9DEBA5ACD8D}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M58" sqref="M58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
-    <col min="2" max="2" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="8"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="8"/>
+    <col min="4" max="4" width="8.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -996,8 +1384,29 @@
       <c r="D1" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1010,9 +1419,32 @@
       <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1025,9 +1457,32 @@
       <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1040,9 +1495,32 @@
       <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1055,8 +1533,32 @@
       <c r="D5" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1069,8 +1571,32 @@
       <c r="D6" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1083,92 +1609,260 @@
       <c r="D7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="10" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="10" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="E10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="15" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="E11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="15" t="s">
         <v>51</v>
       </c>
       <c r="D12" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="E12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="15" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1181,8 +1875,32 @@
       <c r="D14" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L14">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -1195,8 +1913,32 @@
       <c r="D15" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15" s="5">
+        <v>110</v>
+      </c>
+      <c r="F15" s="5">
+        <v>110</v>
+      </c>
+      <c r="G15" s="5">
+        <v>110</v>
+      </c>
+      <c r="H15" s="5">
+        <v>110</v>
+      </c>
+      <c r="I15" s="5">
+        <v>110</v>
+      </c>
+      <c r="J15" s="5">
+        <v>110</v>
+      </c>
+      <c r="K15" s="5">
+        <v>110</v>
+      </c>
+      <c r="L15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -1209,8 +1951,32 @@
       <c r="D16" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="5">
+        <v>38</v>
+      </c>
+      <c r="F16" s="5">
+        <v>38</v>
+      </c>
+      <c r="G16" s="5">
+        <v>38</v>
+      </c>
+      <c r="H16" s="5">
+        <v>38</v>
+      </c>
+      <c r="I16" s="5">
+        <v>38</v>
+      </c>
+      <c r="J16" s="5">
+        <v>38</v>
+      </c>
+      <c r="K16" s="5">
+        <v>38</v>
+      </c>
+      <c r="L16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -1223,8 +1989,32 @@
       <c r="D17" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="5">
+        <v>126</v>
+      </c>
+      <c r="F17" s="5">
+        <v>126</v>
+      </c>
+      <c r="G17" s="5">
+        <v>126</v>
+      </c>
+      <c r="H17" s="5">
+        <v>126</v>
+      </c>
+      <c r="I17" s="5">
+        <v>126</v>
+      </c>
+      <c r="J17" s="5">
+        <v>126</v>
+      </c>
+      <c r="K17" s="5">
+        <v>126</v>
+      </c>
+      <c r="L17">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>121</v>
       </c>
@@ -1237,8 +2027,32 @@
       <c r="D18" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="5">
+        <v>204</v>
+      </c>
+      <c r="F18" s="5">
+        <v>204</v>
+      </c>
+      <c r="G18" s="5">
+        <v>204</v>
+      </c>
+      <c r="H18" s="5">
+        <v>204</v>
+      </c>
+      <c r="I18" s="5">
+        <v>204</v>
+      </c>
+      <c r="J18" s="5">
+        <v>204</v>
+      </c>
+      <c r="K18" s="5">
+        <v>204</v>
+      </c>
+      <c r="L18">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -1251,8 +2065,32 @@
       <c r="D19" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="5">
+        <v>60</v>
+      </c>
+      <c r="F19" s="5">
+        <v>60</v>
+      </c>
+      <c r="G19" s="5">
+        <v>60</v>
+      </c>
+      <c r="H19" s="5">
+        <v>60</v>
+      </c>
+      <c r="I19" s="5">
+        <v>60</v>
+      </c>
+      <c r="J19" s="5">
+        <v>60</v>
+      </c>
+      <c r="K19" s="5">
+        <v>60</v>
+      </c>
+      <c r="L19">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1265,8 +2103,32 @@
       <c r="D20" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J20" s="9">
+        <v>1</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L20">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1279,8 +2141,32 @@
       <c r="D21" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="9">
+        <v>1</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1293,8 +2179,32 @@
       <c r="D22" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>123</v>
       </c>
@@ -1307,8 +2217,32 @@
       <c r="D23" s="3">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="9">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -1321,8 +2255,32 @@
       <c r="D24" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="9">
+        <v>1</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L24">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>125</v>
       </c>
@@ -1335,8 +2293,32 @@
       <c r="D25" s="3">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -1349,8 +2331,32 @@
       <c r="D26" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1363,8 +2369,32 @@
       <c r="D27" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1377,8 +2407,32 @@
       <c r="D28" s="3">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="5">
+        <v>1200</v>
+      </c>
+      <c r="F28" s="10">
+        <v>2000</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1200</v>
+      </c>
+      <c r="H28" s="5">
+        <v>1200</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1200</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1200</v>
+      </c>
+      <c r="K28" s="10">
+        <v>5000</v>
+      </c>
+      <c r="L28">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1391,8 +2445,32 @@
       <c r="D29" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1405,8 +2483,32 @@
       <c r="D30" s="3">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="10">
+        <v>3</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K30" s="10">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -1419,8 +2521,32 @@
       <c r="D31" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" s="8">
+        <v>74</v>
+      </c>
+      <c r="F31" s="8">
+        <v>74</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0</v>
+      </c>
+      <c r="H31" s="8">
+        <v>0</v>
+      </c>
+      <c r="I31" s="8">
+        <v>74</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0</v>
+      </c>
+      <c r="K31" s="8">
+        <v>74</v>
+      </c>
+      <c r="L31" s="8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -1433,8 +2559,32 @@
       <c r="D32" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="8">
+        <v>80</v>
+      </c>
+      <c r="F32" s="8">
+        <v>80</v>
+      </c>
+      <c r="G32" s="8">
+        <v>0</v>
+      </c>
+      <c r="H32" s="8">
+        <v>0</v>
+      </c>
+      <c r="I32" s="8">
+        <v>80</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0</v>
+      </c>
+      <c r="K32" s="8">
+        <v>80</v>
+      </c>
+      <c r="L32" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -1447,8 +2597,32 @@
       <c r="D33" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" s="8">
+        <v>60</v>
+      </c>
+      <c r="F33" s="8">
+        <v>60</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0</v>
+      </c>
+      <c r="H33" s="8">
+        <v>0</v>
+      </c>
+      <c r="I33" s="8">
+        <v>60</v>
+      </c>
+      <c r="J33" s="8">
+        <v>100</v>
+      </c>
+      <c r="K33" s="8">
+        <v>60</v>
+      </c>
+      <c r="L33" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -1461,22 +2635,70 @@
       <c r="D34" s="3">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
+      <c r="E34" s="8">
+        <v>66</v>
+      </c>
+      <c r="F34" s="8">
+        <v>66</v>
+      </c>
+      <c r="G34" s="10">
+        <v>100</v>
+      </c>
+      <c r="H34" s="8">
+        <v>0</v>
+      </c>
+      <c r="I34" s="8">
+        <v>66</v>
+      </c>
+      <c r="J34" s="8">
+        <v>0</v>
+      </c>
+      <c r="K34" s="8">
+        <v>66</v>
+      </c>
+      <c r="L34" s="8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="12">
         <v>64</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="13">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="12">
+        <v>64</v>
+      </c>
+      <c r="F35" s="8">
+        <v>64</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0</v>
+      </c>
+      <c r="H35" s="8">
+        <v>100</v>
+      </c>
+      <c r="I35" s="8">
+        <v>64</v>
+      </c>
+      <c r="J35" s="8">
+        <v>0</v>
+      </c>
+      <c r="K35" s="8">
+        <v>64</v>
+      </c>
+      <c r="L35" s="12">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1489,8 +2711,32 @@
       <c r="D36" s="3">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" s="8">
+        <v>73</v>
+      </c>
+      <c r="F36" s="8">
+        <v>73</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0</v>
+      </c>
+      <c r="H36" s="8">
+        <v>0</v>
+      </c>
+      <c r="I36" s="8">
+        <v>73</v>
+      </c>
+      <c r="J36" s="8">
+        <v>0</v>
+      </c>
+      <c r="K36" s="8">
+        <v>73</v>
+      </c>
+      <c r="L36" s="8">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -1503,8 +2749,32 @@
       <c r="D37" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="8">
+        <v>59</v>
+      </c>
+      <c r="F37" s="8">
+        <v>59</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0</v>
+      </c>
+      <c r="H37" s="8">
+        <v>0</v>
+      </c>
+      <c r="I37" s="8">
+        <v>59</v>
+      </c>
+      <c r="J37" s="8">
+        <v>0</v>
+      </c>
+      <c r="K37" s="8">
+        <v>59</v>
+      </c>
+      <c r="L37" s="8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1517,8 +2787,32 @@
       <c r="D38" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="8">
+        <v>72</v>
+      </c>
+      <c r="F38" s="8">
+        <v>72</v>
+      </c>
+      <c r="G38" s="8">
+        <v>0</v>
+      </c>
+      <c r="H38" s="8">
+        <v>0</v>
+      </c>
+      <c r="I38" s="8">
+        <v>72</v>
+      </c>
+      <c r="J38" s="8">
+        <v>0</v>
+      </c>
+      <c r="K38" s="8">
+        <v>72</v>
+      </c>
+      <c r="L38" s="8">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -1531,8 +2825,32 @@
       <c r="D39" s="3">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" s="8">
+        <v>72</v>
+      </c>
+      <c r="F39" s="8">
+        <v>72</v>
+      </c>
+      <c r="G39" s="8">
+        <v>0</v>
+      </c>
+      <c r="H39" s="8">
+        <v>0</v>
+      </c>
+      <c r="I39" s="8">
+        <v>72</v>
+      </c>
+      <c r="J39" s="8">
+        <v>0</v>
+      </c>
+      <c r="K39" s="8">
+        <v>72</v>
+      </c>
+      <c r="L39" s="8">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>74</v>
       </c>
@@ -1545,8 +2863,32 @@
       <c r="D40" s="3">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" s="8">
+        <v>24</v>
+      </c>
+      <c r="F40" s="8">
+        <v>24</v>
+      </c>
+      <c r="G40" s="8">
+        <v>0</v>
+      </c>
+      <c r="H40" s="8">
+        <v>0</v>
+      </c>
+      <c r="I40" s="8">
+        <v>24</v>
+      </c>
+      <c r="J40" s="8">
+        <v>100</v>
+      </c>
+      <c r="K40" s="8">
+        <v>24</v>
+      </c>
+      <c r="L40" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -1559,22 +2901,70 @@
       <c r="D41" s="3">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
+      <c r="E41" s="8">
+        <v>73</v>
+      </c>
+      <c r="F41" s="8">
+        <v>73</v>
+      </c>
+      <c r="G41" s="10">
+        <v>100</v>
+      </c>
+      <c r="H41" s="8">
+        <v>0</v>
+      </c>
+      <c r="I41" s="8">
+        <v>73</v>
+      </c>
+      <c r="J41" s="8">
+        <v>0</v>
+      </c>
+      <c r="K41" s="8">
+        <v>73</v>
+      </c>
+      <c r="L41" s="8">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="12">
         <v>73</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="13">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" s="12">
+        <v>73</v>
+      </c>
+      <c r="F42" s="8">
+        <v>73</v>
+      </c>
+      <c r="G42" s="8">
+        <v>0</v>
+      </c>
+      <c r="H42" s="8">
+        <v>100</v>
+      </c>
+      <c r="I42" s="8">
+        <v>73</v>
+      </c>
+      <c r="J42" s="8">
+        <v>0</v>
+      </c>
+      <c r="K42" s="8">
+        <v>73</v>
+      </c>
+      <c r="L42" s="12">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -1587,8 +2977,32 @@
       <c r="D43" s="3">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" s="8">
+        <v>79</v>
+      </c>
+      <c r="F43" s="8">
+        <v>79</v>
+      </c>
+      <c r="G43" s="8">
+        <v>0</v>
+      </c>
+      <c r="H43" s="8">
+        <v>0</v>
+      </c>
+      <c r="I43" s="8">
+        <v>79</v>
+      </c>
+      <c r="J43" s="8">
+        <v>0</v>
+      </c>
+      <c r="K43" s="8">
+        <v>79</v>
+      </c>
+      <c r="L43" s="8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -1601,8 +3015,32 @@
       <c r="D44" s="3">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="8">
+        <v>61</v>
+      </c>
+      <c r="F44" s="8">
+        <v>61</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0</v>
+      </c>
+      <c r="H44" s="8">
+        <v>0</v>
+      </c>
+      <c r="I44" s="8">
+        <v>61</v>
+      </c>
+      <c r="J44" s="8">
+        <v>0</v>
+      </c>
+      <c r="K44" s="8">
+        <v>61</v>
+      </c>
+      <c r="L44" s="8">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -1615,8 +3053,32 @@
       <c r="D45" s="3">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" s="8">
+        <v>70</v>
+      </c>
+      <c r="F45" s="8">
+        <v>70</v>
+      </c>
+      <c r="G45" s="8">
+        <v>0</v>
+      </c>
+      <c r="H45" s="8">
+        <v>0</v>
+      </c>
+      <c r="I45" s="8">
+        <v>70</v>
+      </c>
+      <c r="J45" s="8">
+        <v>0</v>
+      </c>
+      <c r="K45" s="8">
+        <v>70</v>
+      </c>
+      <c r="L45" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -1629,8 +3091,32 @@
       <c r="D46" s="3">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" s="8">
+        <v>68</v>
+      </c>
+      <c r="F46" s="8">
+        <v>68</v>
+      </c>
+      <c r="G46" s="8">
+        <v>0</v>
+      </c>
+      <c r="H46" s="8">
+        <v>0</v>
+      </c>
+      <c r="I46" s="8">
+        <v>68</v>
+      </c>
+      <c r="J46" s="8">
+        <v>0</v>
+      </c>
+      <c r="K46" s="8">
+        <v>68</v>
+      </c>
+      <c r="L46" s="8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>81</v>
       </c>
@@ -1643,8 +3129,32 @@
       <c r="D47" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" s="8">
+        <v>68</v>
+      </c>
+      <c r="F47" s="8">
+        <v>68</v>
+      </c>
+      <c r="G47" s="8">
+        <v>0</v>
+      </c>
+      <c r="H47" s="8">
+        <v>0</v>
+      </c>
+      <c r="I47" s="8">
+        <v>68</v>
+      </c>
+      <c r="J47" s="8">
+        <v>100</v>
+      </c>
+      <c r="K47" s="8">
+        <v>68</v>
+      </c>
+      <c r="L47" s="8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -1657,22 +3167,70 @@
       <c r="D48" s="3">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
+      <c r="E48" s="8">
+        <v>81</v>
+      </c>
+      <c r="F48" s="8">
+        <v>81</v>
+      </c>
+      <c r="G48" s="10">
+        <v>100</v>
+      </c>
+      <c r="H48" s="8">
+        <v>0</v>
+      </c>
+      <c r="I48" s="8">
+        <v>81</v>
+      </c>
+      <c r="J48" s="8">
+        <v>0</v>
+      </c>
+      <c r="K48" s="8">
+        <v>81</v>
+      </c>
+      <c r="L48" s="8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49" s="12">
         <v>82</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="13">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" s="12">
+        <v>82</v>
+      </c>
+      <c r="F49" s="8">
+        <v>82</v>
+      </c>
+      <c r="G49" s="8">
+        <v>0</v>
+      </c>
+      <c r="H49" s="8">
+        <v>100</v>
+      </c>
+      <c r="I49" s="8">
+        <v>82</v>
+      </c>
+      <c r="J49" s="8">
+        <v>0</v>
+      </c>
+      <c r="K49" s="8">
+        <v>82</v>
+      </c>
+      <c r="L49" s="12">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -1685,8 +3243,32 @@
       <c r="D50" s="3">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" s="8">
+        <v>83</v>
+      </c>
+      <c r="F50" s="8">
+        <v>83</v>
+      </c>
+      <c r="G50" s="8">
+        <v>0</v>
+      </c>
+      <c r="H50" s="8">
+        <v>0</v>
+      </c>
+      <c r="I50" s="8">
+        <v>83</v>
+      </c>
+      <c r="J50" s="8">
+        <v>0</v>
+      </c>
+      <c r="K50" s="8">
+        <v>83</v>
+      </c>
+      <c r="L50" s="8">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -1699,8 +3281,32 @@
       <c r="D51" s="3">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" s="8">
+        <v>62</v>
+      </c>
+      <c r="F51" s="8">
+        <v>62</v>
+      </c>
+      <c r="G51" s="8">
+        <v>0</v>
+      </c>
+      <c r="H51" s="8">
+        <v>0</v>
+      </c>
+      <c r="I51" s="8">
+        <v>62</v>
+      </c>
+      <c r="J51" s="8">
+        <v>0</v>
+      </c>
+      <c r="K51" s="8">
+        <v>62</v>
+      </c>
+      <c r="L51" s="8">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -1713,8 +3319,32 @@
       <c r="D52" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="L52">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -1727,8 +3357,32 @@
       <c r="D53" s="3">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L53">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -1736,13 +3390,37 @@
         <v>88</v>
       </c>
       <c r="C54" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D54" s="3">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" s="8">
+        <v>0</v>
+      </c>
+      <c r="F54" s="8">
+        <v>0</v>
+      </c>
+      <c r="G54" s="8">
+        <v>0</v>
+      </c>
+      <c r="H54" s="8">
+        <v>0</v>
+      </c>
+      <c r="I54" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="J54" s="8">
+        <v>0</v>
+      </c>
+      <c r="K54" s="8">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>142</v>
       </c>
@@ -1755,8 +3433,32 @@
       <c r="D55" s="3">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="L55">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>143</v>
       </c>
@@ -1769,8 +3471,32 @@
       <c r="D56" s="3">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="L56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>144</v>
       </c>
@@ -1783,8 +3509,32 @@
       <c r="D57" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="K57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="L57">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>145</v>
       </c>
@@ -1797,8 +3547,32 @@
       <c r="D58" s="3">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="J58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="L58">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>146</v>
       </c>
@@ -1811,8 +3585,32 @@
       <c r="D59" s="3">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="L59">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>147</v>
       </c>
@@ -1825,8 +3623,32 @@
       <c r="D60" s="3">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="L60">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>148</v>
       </c>
@@ -1839,8 +3661,32 @@
       <c r="D61" s="3">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="L61">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>149</v>
       </c>
@@ -1853,8 +3699,32 @@
       <c r="D62" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="I62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="L62">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>150</v>
       </c>
@@ -1867,8 +3737,32 @@
       <c r="D63" s="3">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I63" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J63" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="K63" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="L63">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>151</v>
       </c>
@@ -1881,8 +3775,32 @@
       <c r="D64" s="3">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L64">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>152</v>
       </c>
@@ -1895,8 +3813,32 @@
       <c r="D65" s="3">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="K65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="L65">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>153</v>
       </c>
@@ -1909,8 +3851,32 @@
       <c r="D66" s="3">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="K66" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="L66">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>154</v>
       </c>
@@ -1923,8 +3889,32 @@
       <c r="D67" s="3">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="I67" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="J67" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="K67" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="L67">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>155</v>
       </c>
@@ -1937,8 +3927,32 @@
       <c r="D68" s="3">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="I68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="J68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L68">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>156</v>
       </c>
@@ -1951,8 +3965,32 @@
       <c r="D69" s="3">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I69" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="K69" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="L69">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>157</v>
       </c>
@@ -1965,8 +4003,32 @@
       <c r="D70" s="3">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="K70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="L70">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>158</v>
       </c>
@@ -1979,8 +4041,32 @@
       <c r="D71" s="3">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="K71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L71">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>159</v>
       </c>
@@ -1992,10 +4078,88 @@
       </c>
       <c r="D72" s="3">
         <v>70</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H72" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="I72" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J72" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K72" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="L72">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0.6</v>
+      </c>
+      <c r="B75">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>0.5</v>
+      </c>
+      <c r="B76">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>0.3</v>
+      </c>
+      <c r="B77">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>0.6</v>
+      </c>
+      <c r="B126">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>0.5</v>
+      </c>
+      <c r="B127">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>0.5</v>
+      </c>
+      <c r="B128">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>